<commit_message>
Added mean curve method1
</commit_message>
<xml_diff>
--- a/master_time_sheet.xlsx
+++ b/master_time_sheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bwedu-my.sharepoint.com/personal/raghavakrishna_devineni_bwedu_de/Documents/5_PythonFiles/Wind Velocities/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bwedu-my.sharepoint.com/personal/raghavakrishna_devineni_bwedu_de/Documents/5_PythonFiles/ESHL_CBo_Post_Processing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="32" documentId="11_F25DC773A252ABDACC104854B11976DA5ADE58F4" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ECAC3524-721F-4B65-B894-8DCDABF43EE6}"/>
+  <xr:revisionPtr revIDLastSave="42" documentId="11_F25DC773A252ABDACC104854B11976DA5ADE58F4" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7622BDB8-B70F-4755-AB19-00939371C129}"/>
   <bookViews>
-    <workbookView xWindow="-19310" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="34">
   <si>
     <t>experiment</t>
   </si>
@@ -109,6 +109,24 @@
   </si>
   <si>
     <t>cbo_winter</t>
+  </si>
+  <si>
+    <t>exclude</t>
+  </si>
+  <si>
+    <t>außen,3l_kü,3l_wz,4l,2l,1l,bd,bd_original</t>
+  </si>
+  <si>
+    <t>außen,3l_kü,3l_wz,4l,2l,1l</t>
+  </si>
+  <si>
+    <t>1a,1l,2l,3l,4a_testo,4l,außen</t>
+  </si>
+  <si>
+    <t>1l,1a_testo,1t,2a_testo,2l,3l,4a_testo,4l,außen</t>
+  </si>
+  <si>
+    <t>1a,1l,1l_sub,2l,3f,3l,4a,4a_sub,4a_testo,4l,5flur,5treppe,außen,tr,weather</t>
   </si>
 </sst>
 </file>
@@ -443,10 +461,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -454,9 +472,10 @@
     <col min="1" max="1" width="35.140625" customWidth="1"/>
     <col min="2" max="3" width="18.5703125" customWidth="1"/>
     <col min="4" max="4" width="22.7109375" customWidth="1"/>
+    <col min="5" max="5" width="68" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -469,8 +488,11 @@
       <c r="D1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -483,8 +505,11 @@
       <c r="D2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -497,8 +522,11 @@
       <c r="D3" s="5" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -511,8 +539,11 @@
       <c r="D4" s="5" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -525,8 +556,11 @@
       <c r="D5" s="5" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -539,8 +573,11 @@
       <c r="D6" s="5" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -553,8 +590,11 @@
       <c r="D7" s="5" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>9</v>
       </c>
@@ -567,8 +607,11 @@
       <c r="D8" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>10</v>
       </c>
@@ -581,8 +624,11 @@
       <c r="D9" s="5" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>11</v>
       </c>
@@ -595,8 +641,11 @@
       <c r="D10" s="5" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>12</v>
       </c>
@@ -609,8 +658,11 @@
       <c r="D11" s="5" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>13</v>
       </c>
@@ -623,8 +675,11 @@
       <c r="D12" s="5" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E12" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>14</v>
       </c>
@@ -637,8 +692,11 @@
       <c r="D13" s="5" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E13" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>15</v>
       </c>
@@ -651,8 +709,11 @@
       <c r="D14" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E14" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>16</v>
       </c>
@@ -665,8 +726,11 @@
       <c r="D15" s="5" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>17</v>
       </c>
@@ -679,8 +743,11 @@
       <c r="D16" s="5" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E16" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>18</v>
       </c>
@@ -693,8 +760,11 @@
       <c r="D17" s="5" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E17" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
         <v>19</v>
       </c>
@@ -707,8 +777,11 @@
       <c r="D18" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E18" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
         <v>20</v>
       </c>
@@ -721,8 +794,11 @@
       <c r="D19" s="5" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E19" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
         <v>21</v>
       </c>
@@ -735,8 +811,11 @@
       <c r="D20" s="5" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E20" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
         <v>22</v>
       </c>
@@ -748,6 +827,9 @@
       </c>
       <c r="D21" s="5" t="s">
         <v>27</v>
+      </c>
+      <c r="E21" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed curve delta CO2
</commit_message>
<xml_diff>
--- a/master_time_sheet.xlsx
+++ b/master_time_sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bwedu-my.sharepoint.com/personal/raghavakrishna_devineni_bwedu_de/Documents/5_PythonFiles/ESHL_CBo_Post_Processing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="42" documentId="11_F25DC773A252ABDACC104854B11976DA5ADE58F4" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7622BDB8-B70F-4755-AB19-00939371C129}"/>
+  <xr:revisionPtr revIDLastSave="60" documentId="11_F25DC773A252ABDACC104854B11976DA5ADE58F4" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{014112D1-0C84-4A64-A265-5D6306F73821}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,8 +24,67 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Raghavakrishna Devineni</author>
+  </authors>
+  <commentList>
+    <comment ref="A14" authorId="0" shapeId="0" xr:uid="{8A79E6C1-33B4-4E6F-A3D1-19F3D8A6450F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Raghavakrishna Devineni:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+No outdoor CO2 data</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A15" authorId="0" shapeId="0" xr:uid="{317B253A-517F-4BE3-96BE-F016036EDA22}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Raghavakrishna Devineni:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+No outdoor CO2 data
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="38">
   <si>
     <t>experiment</t>
   </si>
@@ -127,6 +186,18 @@
   </si>
   <si>
     <t>1a,1l,1l_sub,2l,3f,3l,4a,4a_sub,4a_testo,4l,5flur,5treppe,außen,tr,weather</t>
+  </si>
+  <si>
+    <t>calibration</t>
+  </si>
+  <si>
+    <t>eshl_calibration</t>
+  </si>
+  <si>
+    <t>cbo_calibration</t>
+  </si>
+  <si>
+    <t>außen,3l_kü,3l_wz,4l,2l,1l,bd,bd_original,</t>
   </si>
 </sst>
 </file>
@@ -136,7 +207,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy/mm/dd\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -150,13 +221,32 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -171,7 +261,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -181,6 +271,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -460,11 +551,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="F8" sqref="F8:F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -473,9 +564,10 @@
     <col min="2" max="3" width="18.5703125" customWidth="1"/>
     <col min="4" max="4" width="22.7109375" customWidth="1"/>
     <col min="5" max="5" width="68" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -491,8 +583,11 @@
       <c r="E1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -506,10 +601,13 @@
         <v>24</v>
       </c>
       <c r="E2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+      <c r="F2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -525,8 +623,11 @@
       <c r="E3" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -542,8 +643,11 @@
       <c r="E4" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -559,8 +663,11 @@
       <c r="E5" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -576,8 +683,11 @@
       <c r="E6" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -593,8 +703,11 @@
       <c r="E7" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F7" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>9</v>
       </c>
@@ -610,8 +723,11 @@
       <c r="E8" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F8" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>10</v>
       </c>
@@ -627,8 +743,11 @@
       <c r="E9" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F9" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>11</v>
       </c>
@@ -644,8 +763,11 @@
       <c r="E10" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F10" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>12</v>
       </c>
@@ -661,8 +783,11 @@
       <c r="E11" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F11" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>13</v>
       </c>
@@ -678,8 +803,11 @@
       <c r="E12" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F12" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>14</v>
       </c>
@@ -695,9 +823,12 @@
       <c r="E13" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
+      <c r="F13" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="9" t="s">
         <v>15</v>
       </c>
       <c r="B14" s="6">
@@ -712,9 +843,12 @@
       <c r="E14" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
+      <c r="F14" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="9" t="s">
         <v>16</v>
       </c>
       <c r="B15" s="6">
@@ -729,8 +863,11 @@
       <c r="E15" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F15" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>17</v>
       </c>
@@ -746,8 +883,11 @@
       <c r="E16" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F16" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>18</v>
       </c>
@@ -763,8 +903,11 @@
       <c r="E17" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F17" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
         <v>19</v>
       </c>
@@ -780,8 +923,11 @@
       <c r="E18" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F18" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
         <v>20</v>
       </c>
@@ -797,8 +943,11 @@
       <c r="E19" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F19" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
         <v>21</v>
       </c>
@@ -814,8 +963,11 @@
       <c r="E20" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F20" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
         <v>22</v>
       </c>
@@ -830,10 +982,14 @@
       </c>
       <c r="E21" t="s">
         <v>33</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>